<commit_message>
Make menu accept first character of cheat code typed, give visual feedback if it's been entered correctly
</commit_message>
<xml_diff>
--- a/src/docs/Levels.xlsx
+++ b/src/docs/Levels.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\GitRepos\CodeGarden\codegarden\src\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\apenkooi\codegarden\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -64,10 +64,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -647,10 +647,10 @@
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1156,7 +1156,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,7 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="51"/>
+      <c r="O10" s="22"/>
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1370,7 +1370,7 @@
       <c r="M12" s="41"/>
       <c r="N12" s="56"/>
       <c r="O12" s="8"/>
-      <c r="P12" s="10"/>
+      <c r="P12" s="51"/>
       <c r="T12" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>